<commit_message>
Final commit of ACO Test to get file for appendix
</commit_message>
<xml_diff>
--- a/Financial Forecast.xlsx
+++ b/Financial Forecast.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/kk19332_bristol_ac_uk/Documents/Documents/Eng Des/Year 5/BioAI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{558E0E5A-7F16-452E-BF85-767A89E35A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="108" documentId="8_{558E0E5A-7F16-452E-BF85-767A89E35A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C3DEEF0-EF2C-41AB-AFB0-2381C02B8253}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="25920" windowHeight="16629" xr2:uid="{538EFC3A-09D1-4104-AE9A-3173A2155281}"/>
+    <workbookView xWindow="7509" yWindow="2589" windowWidth="10122" windowHeight="3300" xr2:uid="{538EFC3A-09D1-4104-AE9A-3173A2155281}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
   <si>
     <t>Revenue</t>
   </si>
@@ -92,9 +92,6 @@
     <t>Data Acquisition per Year</t>
   </si>
   <si>
-    <t>Total Cost</t>
-  </si>
-  <si>
     <t>Total Profit</t>
   </si>
   <si>
@@ -102,6 +99,12 @@
   </si>
   <si>
     <t>Cashflow</t>
+  </si>
+  <si>
+    <t>Total Outgoings</t>
+  </si>
+  <si>
+    <t>Total Income</t>
   </si>
 </sst>
 </file>
@@ -128,15 +131,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -144,25 +159,273 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -264,7 +527,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Total Revenue</c:v>
+                  <c:v>Total Income</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -317,19 +580,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>130000</c:v>
+                  <c:v>250000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>260000</c:v>
+                  <c:v>1055000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>360000</c:v>
+                  <c:v>3205000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>430000</c:v>
+                  <c:v>9600000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -346,11 +609,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$20</c:f>
+              <c:f>Sheet1!$A$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Total Cost</c:v>
+                  <c:v>Total Outgoings</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -403,19 +666,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>141700</c:v>
+                  <c:v>184700</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>170700</c:v>
+                  <c:v>451400</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>240700</c:v>
+                  <c:v>703400</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>230700</c:v>
+                  <c:v>1297400</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>230700</c:v>
+                  <c:v>2121400</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -424,92 +687,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-B6F8-441D-A27C-82C599D4EAAA}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$21</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Total Profit</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$18:$G$18</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Year 0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Year 1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Year 2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Year 3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Year 4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Year 5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$21:$G$21</c:f>
-              <c:numCache>
-                <c:formatCode>"£"#,##0_);[Red]\("£"#,##0\)</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-126700</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-40700</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>19300</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>129300</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>199300</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-B6F8-441D-A27C-82C599D4EAAA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -575,19 +752,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-126700</c:v>
+                  <c:v>-184700</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-167400</c:v>
+                  <c:v>-201400</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-21400</c:v>
+                  <c:v>351600</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>148600</c:v>
+                  <c:v>1907600</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>328600</c:v>
+                  <c:v>7478600</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -595,7 +772,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-B6F8-441D-A27C-82C599D4EAAA}"/>
+              <c16:uniqueId val="{00000006-6FD7-4260-9ACA-3861BD19FB8D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -610,6 +787,116 @@
         <c:smooth val="0"/>
         <c:axId val="414195311"/>
         <c:axId val="1031046319"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$21</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Total Profit</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$18:$G$18</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>Year 0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Year 1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Year 2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Year 3</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>Year 4</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Year 5</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$21:$G$21</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>"£"#,##0_);[Red]\("£"#,##0\)</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0" formatCode="General">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>-184700</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>-16700</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>368300</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1539300</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>5939300</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-B6F8-441D-A27C-82C599D4EAAA}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
       </c:lineChart>
       <c:catAx>
         <c:axId val="414195311"/>
@@ -1364,13 +1651,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>312964</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>103414</xdr:rowOff>
+      <xdr:rowOff>103413</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>97971</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>44941</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>60476</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1697,392 +1984,458 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEBA9B6D-4A5D-431D-BEEF-DC26FFFDBBAD}">
   <dimension ref="A2:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="69" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="32.69140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.69140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="9.84375" customWidth="1"/>
+    <col min="6" max="6" width="9.84375" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="9.84375" customWidth="1"/>
+    <col min="12" max="12" width="9.84375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="C2" s="1" t="s">
+    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
+      <c r="D3" s="31"/>
+      <c r="E3" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1" t="s">
+      <c r="F3" s="33"/>
+      <c r="G3" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
+      <c r="H3" s="31"/>
+      <c r="I3" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1" t="s">
+      <c r="J3" s="33"/>
+      <c r="K3" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="1"/>
+      <c r="L3" s="31"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B3" t="s">
+    <row r="4" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L4" s="10" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A4" s="4" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="27">
         <v>3000</v>
       </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5" s="5">
+      <c r="C5" s="13">
+        <v>0</v>
+      </c>
+      <c r="D5" s="14">
         <f>C5*$B5</f>
-        <v>15000</v>
-      </c>
-      <c r="E5">
-        <v>20</v>
-      </c>
-      <c r="F5" s="5">
-        <f t="shared" ref="F5:L5" si="0">E5*$B5</f>
-        <v>60000</v>
-      </c>
-      <c r="G5">
-        <v>40</v>
-      </c>
-      <c r="H5" s="5">
-        <f t="shared" ref="H5:L5" si="1">G5*$B5</f>
-        <v>120000</v>
-      </c>
-      <c r="I5">
-        <v>50</v>
-      </c>
-      <c r="J5" s="5">
-        <f t="shared" ref="J5:L5" si="2">I5*$B5</f>
-        <v>150000</v>
-      </c>
-      <c r="K5">
-        <v>50</v>
-      </c>
-      <c r="L5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="15">
+        <v>25</v>
+      </c>
+      <c r="F5" s="16">
+        <f t="shared" ref="F5" si="0">E5*$B5</f>
+        <v>75000</v>
+      </c>
+      <c r="G5" s="13">
+        <v>35</v>
+      </c>
+      <c r="H5" s="14">
+        <f t="shared" ref="H5" si="1">G5*$B5</f>
+        <v>105000</v>
+      </c>
+      <c r="I5" s="17">
+        <v>100</v>
+      </c>
+      <c r="J5" s="18">
+        <f t="shared" ref="J5" si="2">I5*$B5</f>
+        <v>300000</v>
+      </c>
+      <c r="K5" s="13">
+        <v>300</v>
+      </c>
+      <c r="L5" s="14">
         <f t="shared" ref="L5:L6" si="3">K5*$B5</f>
-        <v>150000</v>
+        <v>900000</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="27">
         <v>7000</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="13">
         <v>0</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="14">
         <f>C6*$B6</f>
         <v>0</v>
       </c>
-      <c r="E6">
-        <v>10</v>
-      </c>
-      <c r="F6" s="5">
-        <f t="shared" ref="F6:L6" si="4">E6*$B6</f>
-        <v>70000</v>
-      </c>
-      <c r="G6">
-        <v>20</v>
-      </c>
-      <c r="H6" s="5">
-        <f t="shared" ref="H6:L6" si="5">G6*$B6</f>
-        <v>140000</v>
-      </c>
-      <c r="I6">
-        <v>30</v>
-      </c>
-      <c r="J6" s="5">
-        <f t="shared" ref="J6:L6" si="6">I6*$B6</f>
-        <v>210000</v>
-      </c>
-      <c r="K6">
-        <v>40</v>
-      </c>
-      <c r="L6" s="5">
+      <c r="E6" s="15">
+        <v>25</v>
+      </c>
+      <c r="F6" s="16">
+        <f t="shared" ref="F6" si="4">E6*$B6</f>
+        <v>175000</v>
+      </c>
+      <c r="G6" s="13">
+        <v>100</v>
+      </c>
+      <c r="H6" s="14">
+        <f t="shared" ref="H6" si="5">G6*$B6</f>
+        <v>700000</v>
+      </c>
+      <c r="I6" s="17">
+        <v>300</v>
+      </c>
+      <c r="J6" s="18">
+        <f t="shared" ref="J6" si="6">I6*$B6</f>
+        <v>2100000</v>
+      </c>
+      <c r="K6" s="13">
+        <v>900</v>
+      </c>
+      <c r="L6" s="14">
         <f t="shared" si="3"/>
-        <v>280000</v>
+        <v>6300000</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
+      <c r="B7" s="28"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="20"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="27">
         <v>5000</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="13">
         <v>1</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="14">
         <f>C8*$B8</f>
         <v>5000</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="17">
         <v>0</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="18">
         <f>E8*$B8</f>
         <v>0</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="13">
         <v>1</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="14">
         <f>G8*$B8</f>
         <v>5000</v>
       </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8" s="5">
+      <c r="I8" s="17">
+        <v>1</v>
+      </c>
+      <c r="J8" s="18">
         <f>I8*$B8</f>
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8" s="5">
+        <v>5000</v>
+      </c>
+      <c r="K8" s="13">
+        <v>1</v>
+      </c>
+      <c r="L8" s="14">
         <f>K8*$B8</f>
-        <v>0</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="27">
         <v>5000</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="13">
         <v>1</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="14">
         <f t="shared" ref="D9:D12" si="7">C9*$B9</f>
         <v>5000</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="17">
         <v>0</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="18">
         <f t="shared" ref="F9:F12" si="8">E9*$B9</f>
         <v>0</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="13">
         <v>1</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="14">
         <f t="shared" ref="H9:H12" si="9">G9*$B9</f>
         <v>5000</v>
       </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9" s="5">
+      <c r="I9" s="17">
+        <v>1</v>
+      </c>
+      <c r="J9" s="18">
         <f t="shared" ref="J9:J12" si="10">I9*$B9</f>
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9" s="5">
+        <v>5000</v>
+      </c>
+      <c r="K9" s="13">
+        <v>1</v>
+      </c>
+      <c r="L9" s="14">
         <f t="shared" ref="L9:L12" si="11">K9*$B9</f>
-        <v>0</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="27">
         <v>2700</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="13">
         <v>1</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="14">
         <f t="shared" si="7"/>
         <v>2700</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="17">
         <v>1</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="18">
         <f t="shared" si="8"/>
         <v>2700</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="13">
         <v>1</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="14">
         <f t="shared" si="9"/>
         <v>2700</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="17">
         <v>1</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10" s="18">
         <f t="shared" si="10"/>
         <v>2700</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="13">
         <v>1</v>
       </c>
-      <c r="L10" s="5">
+      <c r="L10" s="14">
         <f t="shared" si="11"/>
         <v>2700</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="5">
-        <v>30000</v>
-      </c>
-      <c r="C11">
+      <c r="B11" s="27">
+        <v>40000</v>
+      </c>
+      <c r="C11" s="13">
         <v>4</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="14">
         <f t="shared" si="7"/>
-        <v>120000</v>
-      </c>
-      <c r="E11">
-        <v>5</v>
-      </c>
-      <c r="F11" s="5">
+        <v>160000</v>
+      </c>
+      <c r="E11" s="17">
+        <v>6</v>
+      </c>
+      <c r="F11" s="18">
         <f t="shared" si="8"/>
-        <v>150000</v>
-      </c>
-      <c r="G11">
-        <v>7</v>
-      </c>
-      <c r="H11" s="5">
+        <v>240000</v>
+      </c>
+      <c r="G11" s="13">
+        <v>10</v>
+      </c>
+      <c r="H11" s="14">
         <f t="shared" si="9"/>
-        <v>210000</v>
-      </c>
-      <c r="I11">
-        <v>7</v>
-      </c>
-      <c r="J11" s="5">
+        <v>400000</v>
+      </c>
+      <c r="I11" s="17">
+        <v>20</v>
+      </c>
+      <c r="J11" s="18">
         <f t="shared" si="10"/>
-        <v>210000</v>
-      </c>
-      <c r="K11">
-        <v>7</v>
-      </c>
-      <c r="L11" s="5">
+        <v>800000</v>
+      </c>
+      <c r="K11" s="13">
+        <v>30</v>
+      </c>
+      <c r="L11" s="14">
         <f t="shared" si="11"/>
-        <v>210000</v>
+        <v>1200000</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="5">
-        <v>1500</v>
-      </c>
-      <c r="C12">
+      <c r="B12" s="29">
+        <v>2000</v>
+      </c>
+      <c r="C12" s="23">
         <v>6</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="24">
         <f t="shared" si="7"/>
-        <v>9000</v>
-      </c>
-      <c r="E12">
+        <v>12000</v>
+      </c>
+      <c r="E12" s="25">
         <v>12</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="26">
         <f t="shared" si="8"/>
-        <v>18000</v>
-      </c>
-      <c r="G12">
+        <v>24000</v>
+      </c>
+      <c r="G12" s="23">
         <v>12</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="24">
         <f t="shared" si="9"/>
-        <v>18000</v>
-      </c>
-      <c r="I12">
-        <v>12</v>
-      </c>
-      <c r="J12" s="5">
+        <v>24000</v>
+      </c>
+      <c r="I12" s="25">
+        <v>24</v>
+      </c>
+      <c r="J12" s="26">
         <f t="shared" si="10"/>
-        <v>18000</v>
-      </c>
-      <c r="K12">
-        <v>12</v>
-      </c>
-      <c r="L12" s="5">
+        <v>48000</v>
+      </c>
+      <c r="K12" s="23">
+        <v>24</v>
+      </c>
+      <c r="L12" s="24">
         <f t="shared" si="11"/>
-        <v>18000</v>
+        <v>48000</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A13" s="3"/>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16" s="2">
+        <f>SUM(D5:D6)</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="2">
+        <f>SUM(F5:F6)</f>
+        <v>250000</v>
+      </c>
+      <c r="E16" s="2">
+        <f>SUM(H5:H6)</f>
+        <v>805000</v>
+      </c>
+      <c r="F16" s="2">
+        <f>SUM(J5:J6)</f>
+        <v>2400000</v>
+      </c>
+      <c r="G16" s="2">
+        <f>SUM(L5:L6)</f>
+        <v>7200000</v>
+      </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A14" s="3"/>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17" s="2">
+        <f>SUM(D8:D12)</f>
+        <v>184700</v>
+      </c>
+      <c r="D17" s="2">
+        <f>SUM(F8:F12)</f>
+        <v>266700</v>
+      </c>
+      <c r="E17" s="2">
+        <f>SUM(H8:H12)</f>
+        <v>436700</v>
+      </c>
+      <c r="F17" s="2">
+        <f>SUM(J8:J12)</f>
+        <v>860700</v>
+      </c>
+      <c r="G17" s="2">
+        <f>SUM(L8:L12)</f>
+        <v>1260700</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
         <v>3</v>
@@ -2101,125 +2454,127 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A19" s="3" t="s">
-        <v>10</v>
+      <c r="A19" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="B19">
+        <f>B16</f>
         <v>0</v>
       </c>
-      <c r="C19" s="5">
-        <f>SUM(D5:D6)</f>
-        <v>15000</v>
-      </c>
-      <c r="D19" s="5">
-        <f>SUM(F5:F6)</f>
-        <v>130000</v>
-      </c>
-      <c r="E19" s="5">
-        <f>SUM(H5:H6)</f>
-        <v>260000</v>
-      </c>
-      <c r="F19" s="5">
-        <f>SUM(J5:J6)</f>
-        <v>360000</v>
-      </c>
-      <c r="G19" s="5">
-        <f>SUM(L5:L6)</f>
-        <v>430000</v>
+      <c r="C19" s="2">
+        <f>B16+C16</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="2">
+        <f t="shared" ref="D19:G19" si="12">C16+D16</f>
+        <v>250000</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" si="12"/>
+        <v>1055000</v>
+      </c>
+      <c r="F19" s="2">
+        <f t="shared" si="12"/>
+        <v>3205000</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="12"/>
+        <v>9600000</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A20" s="3" t="s">
-        <v>18</v>
+      <c r="A20" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="B20">
+        <f>B17</f>
         <v>0</v>
       </c>
-      <c r="C20" s="5">
-        <f>SUM(D8:D12)</f>
-        <v>141700</v>
-      </c>
-      <c r="D20" s="5">
-        <f>SUM(F8:F12)</f>
-        <v>170700</v>
-      </c>
-      <c r="E20" s="5">
-        <f>SUM(H8:H12)</f>
-        <v>240700</v>
-      </c>
-      <c r="F20" s="5">
-        <f>SUM(J8:J12)</f>
-        <v>230700</v>
-      </c>
-      <c r="G20" s="5">
-        <f>SUM(L8:L12)</f>
-        <v>230700</v>
+      <c r="C20" s="2">
+        <f>B17+C17</f>
+        <v>184700</v>
+      </c>
+      <c r="D20" s="2">
+        <f t="shared" ref="D20:G20" si="13">C17+D17</f>
+        <v>451400</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" si="13"/>
+        <v>703400</v>
+      </c>
+      <c r="F20" s="2">
+        <f t="shared" si="13"/>
+        <v>1297400</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="13"/>
+        <v>2121400</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A21" s="2" t="s">
-        <v>19</v>
+      <c r="A21" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
-      <c r="C21" s="5">
-        <f>C19-C20</f>
-        <v>-126700</v>
-      </c>
-      <c r="D21" s="5">
-        <f>D19-D20</f>
-        <v>-40700</v>
-      </c>
-      <c r="E21" s="5">
-        <f>E19-E20</f>
-        <v>19300</v>
-      </c>
-      <c r="F21" s="5">
-        <f>F19-F20</f>
-        <v>129300</v>
-      </c>
-      <c r="G21" s="5">
-        <f>G19-G20</f>
-        <v>199300</v>
+      <c r="C21" s="2">
+        <f>C16-C17</f>
+        <v>-184700</v>
+      </c>
+      <c r="D21" s="2">
+        <f>D16-D17</f>
+        <v>-16700</v>
+      </c>
+      <c r="E21" s="2">
+        <f>E16-E17</f>
+        <v>368300</v>
+      </c>
+      <c r="F21" s="2">
+        <f>F16-F17</f>
+        <v>1539300</v>
+      </c>
+      <c r="G21" s="2">
+        <f>G16-G17</f>
+        <v>5939300</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A22" s="2" t="s">
-        <v>21</v>
+      <c r="A22" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="B22">
         <v>0</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="2">
         <f>B21+C21</f>
-        <v>-126700</v>
-      </c>
-      <c r="D22" s="5">
+        <v>-184700</v>
+      </c>
+      <c r="D22" s="2">
         <f>C21+D21</f>
-        <v>-167400</v>
-      </c>
-      <c r="E22" s="5">
+        <v>-201400</v>
+      </c>
+      <c r="E22" s="2">
         <f>D21+E21</f>
-        <v>-21400</v>
-      </c>
-      <c r="F22" s="5">
+        <v>351600</v>
+      </c>
+      <c r="F22" s="2">
         <f>E21+F21</f>
-        <v>148600</v>
-      </c>
-      <c r="G22" s="5">
+        <v>1907600</v>
+      </c>
+      <c r="G22" s="2">
         <f>F21+G21</f>
-        <v>328600</v>
-      </c>
-      <c r="H22" s="5"/>
+        <v>7478600</v>
+      </c>
+      <c r="H22" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>